<commit_message>
Parts list Excel files
</commit_message>
<xml_diff>
--- a/KiCad_files/MusselGapeTracker_RevH/MusselGapeTracker_RevH_parts_list.xlsx
+++ b/KiCad_files/MusselGapeTracker_RevH/MusselGapeTracker_RevH_parts_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Hardware_projects\MusselGapeTracker_hardware\KiCad_files\MusselGapeTracker_RevH\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF1A125F-A683-4C39-89C1-455E2B0C2706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD93A51B-BD97-4CA2-B6E7-B1695BBF3334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5750" yWindow="1370" windowWidth="29620" windowHeight="19530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34000" yWindow="830" windowWidth="23270" windowHeight="19070" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="MusselGapeTracker_RevH" sheetId="2" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="436">
   <si>
     <t>Part Description</t>
   </si>
@@ -1017,9 +1017,6 @@
     <t>TE Connectivity Raychem Cable Protection</t>
   </si>
   <si>
-    <t>Heat shrink tubing, 0.315" ID before, 0.079" after, adhesive lined 4ft length (inner layer)</t>
-  </si>
-  <si>
     <t>DWFR-8/2-0-STK-ND</t>
   </si>
   <si>
@@ -1378,6 +1375,24 @@
   </si>
   <si>
     <t>MusselGapeTracker_RevH circuit board (order of 3)</t>
+  </si>
+  <si>
+    <t>Heat shrink 1/4" ID x 4ft - moisture proof adhesive lined, semi-rigid</t>
+  </si>
+  <si>
+    <t>SCL-1/4-0-STK</t>
+  </si>
+  <si>
+    <t>SCL-1/4-0-STK-ND</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>4061T228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O-ring 1/8 width dash number 206 - McMasterCarr pk 100 https://www.mcmaster.com/4061t228/ </t>
   </si>
 </sst>
 </file>
@@ -1678,9 +1693,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1718,7 +1733,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1824,7 +1839,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1966,7 +1981,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1985,11 +2000,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M72"/>
+  <dimension ref="A1:M74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
+      <pane ySplit="2" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2006,7 +2021,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="15" customFormat="1" x14ac:dyDescent="0.35">
@@ -2035,19 +2050,19 @@
         <v>12</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="J2" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="K2" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="K2" s="15" t="s">
-        <v>350</v>
-      </c>
       <c r="L2" s="15" t="s">
+        <v>352</v>
+      </c>
+      <c r="M2" s="15" t="s">
         <v>353</v>
-      </c>
-      <c r="M2" s="15" t="s">
-        <v>354</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="29" x14ac:dyDescent="0.35">
@@ -2349,22 +2364,22 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B14" t="s">
         <v>40</v>
       </c>
       <c r="C14" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E14" s="7">
         <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G14" s="6">
         <v>0.5</v>
@@ -2374,16 +2389,16 @@
         <v>0.5</v>
       </c>
       <c r="J14" t="s">
+        <v>350</v>
+      </c>
+      <c r="K14" t="s">
         <v>351</v>
       </c>
-      <c r="K14" t="s">
-        <v>352</v>
-      </c>
       <c r="L14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="M14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.35">
@@ -2442,19 +2457,19 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C17" t="s">
         <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E17" s="7">
         <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G17" s="6">
         <v>9.7100000000000009</v>
@@ -2464,10 +2479,10 @@
         <v>9.7100000000000009</v>
       </c>
       <c r="J17" t="s">
+        <v>422</v>
+      </c>
+      <c r="K17" t="s">
         <v>423</v>
-      </c>
-      <c r="K17" t="s">
-        <v>424</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
@@ -2596,10 +2611,10 @@
         <v>10</v>
       </c>
       <c r="J22" t="s">
+        <v>360</v>
+      </c>
+      <c r="K22" t="s">
         <v>361</v>
-      </c>
-      <c r="K22" t="s">
-        <v>362</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
@@ -2709,7 +2724,7 @@
     </row>
     <row r="27" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B27" t="s">
         <v>92</v>
@@ -2737,7 +2752,7 @@
         <v>173</v>
       </c>
       <c r="K27" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
@@ -2767,10 +2782,10 @@
         <v>0.38</v>
       </c>
       <c r="J28" t="s">
+        <v>356</v>
+      </c>
+      <c r="K28" t="s">
         <v>357</v>
-      </c>
-      <c r="K28" t="s">
-        <v>358</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
@@ -2790,7 +2805,7 @@
         <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="G29" s="6">
         <v>0.54</v>
@@ -2829,19 +2844,19 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C31" s="37" t="s">
         <v>97</v>
       </c>
       <c r="D31" s="37" t="s">
+        <v>413</v>
+      </c>
+      <c r="E31" s="38">
+        <v>1</v>
+      </c>
+      <c r="F31" s="37" t="s">
         <v>414</v>
-      </c>
-      <c r="E31" s="38">
-        <v>1</v>
-      </c>
-      <c r="F31" s="37" t="s">
-        <v>415</v>
       </c>
       <c r="G31" s="6">
         <v>1.19</v>
@@ -2851,7 +2866,7 @@
         <v>1.19</v>
       </c>
       <c r="I31" s="37" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -2865,13 +2880,13 @@
         <v>93</v>
       </c>
       <c r="D32" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="E32" s="7">
         <v>1</v>
       </c>
       <c r="F32" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G32" s="6">
         <v>2.0699999999999998</v>
@@ -2881,10 +2896,10 @@
         <v>2.0699999999999998</v>
       </c>
       <c r="J32" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="K32" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.35">
@@ -2913,7 +2928,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B34" t="s">
         <v>129</v>
@@ -2940,19 +2955,19 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
+        <v>322</v>
+      </c>
+      <c r="C35" t="s">
+        <v>319</v>
+      </c>
+      <c r="D35" t="s">
         <v>323</v>
       </c>
-      <c r="C35" t="s">
-        <v>320</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" s="7">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
         <v>324</v>
-      </c>
-      <c r="E35" s="7">
-        <v>1</v>
-      </c>
-      <c r="F35" t="s">
-        <v>325</v>
       </c>
       <c r="G35" s="6">
         <v>1.45</v>
@@ -3040,7 +3055,7 @@
         <v>0.16</v>
       </c>
       <c r="I38" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.35">
@@ -3067,7 +3082,7 @@
         <v>0.17</v>
       </c>
       <c r="I39" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -3094,7 +3109,7 @@
         <v>2.3000000000000003</v>
       </c>
       <c r="I40" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.35">
@@ -3170,7 +3185,7 @@
         <v>1.31</v>
       </c>
       <c r="H47" s="6">
-        <f t="shared" ref="H47:H51" si="1">G47*E47</f>
+        <f t="shared" ref="H47:H52" si="1">G47*E47</f>
         <v>20.96</v>
       </c>
     </row>
@@ -3200,19 +3215,19 @@
     </row>
     <row r="49" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
-        <v>310</v>
+        <v>430</v>
       </c>
       <c r="C49" t="s">
         <v>309</v>
       </c>
       <c r="D49" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E49" s="7">
         <v>1</v>
       </c>
       <c r="F49" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="G49" s="6">
         <v>10.81</v>
@@ -3224,19 +3239,19 @@
     </row>
     <row r="50" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C50" t="s">
         <v>309</v>
       </c>
       <c r="D50" t="s">
+        <v>313</v>
+      </c>
+      <c r="E50" s="7">
+        <v>1</v>
+      </c>
+      <c r="F50" t="s">
         <v>314</v>
-      </c>
-      <c r="E50" s="7">
-        <v>1</v>
-      </c>
-      <c r="F50" t="s">
-        <v>315</v>
       </c>
       <c r="G50" s="6">
         <v>7.8</v>
@@ -3246,299 +3261,330 @@
         <v>7.8</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
+        <v>430</v>
+      </c>
+      <c r="C51" t="s">
+        <v>433</v>
+      </c>
+      <c r="D51" t="s">
+        <v>431</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A52" s="4" t="s">
+        <v>326</v>
+      </c>
+      <c r="C52" t="s">
         <v>327</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D52" t="s">
         <v>328</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E52" s="7">
+        <v>1</v>
+      </c>
+      <c r="F52" t="s">
         <v>329</v>
       </c>
-      <c r="E51" s="7">
-        <v>1</v>
-      </c>
-      <c r="F51" t="s">
-        <v>330</v>
-      </c>
-      <c r="G51" s="6">
+      <c r="G52" s="6">
         <v>2.19</v>
       </c>
-      <c r="H51" s="6">
+      <c r="H52" s="6">
         <f t="shared" si="1"/>
         <v>2.19</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A52" s="4" t="s">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A53" s="4" t="s">
+        <v>318</v>
+      </c>
+      <c r="C53" t="s">
         <v>319</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D53" t="s">
         <v>320</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E53" s="7">
+        <v>1</v>
+      </c>
+      <c r="F53" t="s">
         <v>321</v>
       </c>
-      <c r="E52" s="7">
-        <v>1</v>
-      </c>
-      <c r="F52" t="s">
-        <v>322</v>
-      </c>
-      <c r="G52" s="6">
+      <c r="G53" s="6">
         <v>3.51</v>
       </c>
-      <c r="H52" s="6">
-        <f>G52*E52</f>
+      <c r="H53" s="6">
+        <f>G53*E53</f>
         <v>3.51</v>
       </c>
     </row>
-    <row r="54" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A54" s="13" t="s">
+    <row r="54" spans="1:11" ht="30.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="4" t="s">
+        <v>435</v>
+      </c>
+      <c r="C54" t="s">
+        <v>434</v>
+      </c>
+      <c r="D54" t="s">
+        <v>434</v>
+      </c>
+      <c r="E54" s="7">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A56" s="13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="4" t="s">
-        <v>430</v>
-      </c>
-      <c r="C55" s="23" t="s">
+    <row r="57" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="4" t="s">
+        <v>429</v>
+      </c>
+      <c r="C57" s="23" t="s">
+        <v>426</v>
+      </c>
+      <c r="E57" s="7">
+        <v>1</v>
+      </c>
+      <c r="G57" s="11">
+        <v>45.2</v>
+      </c>
+      <c r="H57" s="11">
+        <f>G57/3</f>
+        <v>15.066666666666668</v>
+      </c>
+      <c r="I57" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="C58" s="23" t="s">
+        <v>425</v>
+      </c>
+      <c r="E58" s="7">
+        <v>16</v>
+      </c>
+      <c r="G58" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H58" s="11">
+        <f>G58*E58</f>
+        <v>8</v>
+      </c>
+      <c r="K58" s="39"/>
+    </row>
+    <row r="59" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C59" s="23"/>
+      <c r="G59" s="11"/>
+      <c r="H59" s="11"/>
+    </row>
+    <row r="60" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A60" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="G60" s="11"/>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A61" s="4" t="s">
         <v>427</v>
       </c>
-      <c r="E55" s="7">
-        <v>1</v>
-      </c>
-      <c r="G55" s="11">
-        <v>45.2</v>
-      </c>
-      <c r="H55" s="11">
-        <f>G55/3</f>
-        <v>15.066666666666668</v>
-      </c>
-      <c r="I55" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="56" spans="1:11" ht="28" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="C56" s="23" t="s">
-        <v>426</v>
-      </c>
-      <c r="E56" s="7">
-        <v>16</v>
-      </c>
-      <c r="G56" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="H56" s="11">
-        <f>G56*E56</f>
-        <v>8</v>
-      </c>
-      <c r="K56" s="39"/>
-    </row>
-    <row r="57" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="C57" s="23"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-    </row>
-    <row r="58" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A58" s="13" t="s">
-        <v>118</v>
-      </c>
-      <c r="G58" s="11"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A59" s="4" t="s">
+      <c r="C61" t="s">
+        <v>330</v>
+      </c>
+      <c r="E61" s="7">
+        <v>1</v>
+      </c>
+      <c r="G61" s="11">
+        <v>20</v>
+      </c>
+      <c r="H61" s="11">
+        <f>G61*0</f>
+        <v>0</v>
+      </c>
+      <c r="I61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A62" s="4" t="s">
         <v>428</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C62" t="s">
+        <v>330</v>
+      </c>
+      <c r="E62" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="C63" s="23"/>
+      <c r="G63" s="11"/>
+      <c r="H63" s="11"/>
+    </row>
+    <row r="64" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A64" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E64"/>
+      <c r="F64" s="9" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A65" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="E65" s="7">
+        <v>1</v>
+      </c>
+      <c r="F65" s="36" t="s">
+        <v>411</v>
+      </c>
+      <c r="G65" s="6">
+        <v>9.99</v>
+      </c>
+      <c r="H65" s="6">
+        <f>G65*E65</f>
+        <v>9.99</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A66" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="E66" s="7">
+        <v>1</v>
+      </c>
+      <c r="F66" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="G66" s="6">
+        <v>6.99</v>
+      </c>
+      <c r="H66" s="6">
+        <f t="shared" ref="H66" si="2">G66*E66</f>
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A67"/>
+      <c r="E67"/>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A68"/>
+      <c r="E68"/>
+      <c r="G68" s="19" t="s">
+        <v>335</v>
+      </c>
+      <c r="H68" s="12">
+        <f>SUM(H44:H66,H3:H37)</f>
+        <v>196.5866666666667</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A69" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="E69"/>
+    </row>
+    <row r="70" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>110</v>
+      </c>
+      <c r="E70" s="7">
+        <v>1</v>
+      </c>
+      <c r="F70" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G70" s="6">
+        <v>44.22</v>
+      </c>
+      <c r="H70" s="12">
+        <f>G70*0</f>
+        <v>0</v>
+      </c>
+      <c r="I70" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71" s="4" t="s">
         <v>331</v>
       </c>
-      <c r="E59" s="7">
-        <v>1</v>
-      </c>
-      <c r="G59" s="11">
-        <v>20</v>
-      </c>
-      <c r="H59" s="11">
-        <f>G59*0</f>
-        <v>0</v>
-      </c>
-      <c r="I59" t="s">
+      <c r="C71" t="s">
+        <v>343</v>
+      </c>
+      <c r="D71" t="s">
+        <v>344</v>
+      </c>
+      <c r="E71" s="7">
+        <v>1</v>
+      </c>
+      <c r="F71" t="s">
+        <v>342</v>
+      </c>
+      <c r="G71" s="6">
+        <v>64.5</v>
+      </c>
+      <c r="I71" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A60" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="C60" t="s">
-        <v>331</v>
-      </c>
-      <c r="E60" s="7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="C61" s="23"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-    </row>
-    <row r="62" spans="1:11" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A62" s="13" t="s">
-        <v>109</v>
-      </c>
-      <c r="E62"/>
-      <c r="F62" s="9" t="s">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A72" s="4" t="s">
+        <v>336</v>
+      </c>
+      <c r="C72" t="s">
+        <v>345</v>
+      </c>
+      <c r="D72" t="s">
+        <v>346</v>
+      </c>
+      <c r="E72" s="7">
+        <v>1</v>
+      </c>
+      <c r="F72" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="63" spans="1:11" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A63" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="E63" s="7">
-        <v>1</v>
-      </c>
-      <c r="F63" s="36" t="s">
-        <v>412</v>
-      </c>
-      <c r="G63" s="6">
-        <v>9.99</v>
-      </c>
-      <c r="H63" s="6">
-        <f>G63*E63</f>
-        <v>9.99</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A64" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="E64" s="7">
-        <v>1</v>
-      </c>
-      <c r="F64" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G64" s="6">
-        <v>6.99</v>
-      </c>
-      <c r="H64" s="6">
-        <f t="shared" ref="H64" si="2">G64*E64</f>
-        <v>6.99</v>
-      </c>
-    </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A65"/>
-      <c r="E65"/>
-    </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A66"/>
-      <c r="E66"/>
-      <c r="G66" s="19" t="s">
-        <v>336</v>
-      </c>
-      <c r="H66" s="12">
-        <f>SUM(H44:H64,H3:H37)</f>
-        <v>196.5866666666667</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A67" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="E67"/>
-    </row>
-    <row r="68" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>110</v>
-      </c>
-      <c r="E68" s="7">
-        <v>1</v>
-      </c>
-      <c r="F68" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G68" s="6">
-        <v>44.22</v>
-      </c>
-      <c r="H68" s="12">
-        <f>G68*0</f>
-        <v>0</v>
-      </c>
-      <c r="I68" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A69" s="4" t="s">
-        <v>332</v>
-      </c>
-      <c r="C69" t="s">
-        <v>344</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="G72" s="6">
+        <v>129.94999999999999</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="A73" s="4" t="s">
+        <v>337</v>
+      </c>
+      <c r="C73" t="s">
         <v>345</v>
       </c>
-      <c r="E69" s="7">
-        <v>1</v>
-      </c>
-      <c r="F69" t="s">
-        <v>343</v>
-      </c>
-      <c r="G69" s="6">
-        <v>64.5</v>
-      </c>
-      <c r="I69" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A70" s="4" t="s">
-        <v>337</v>
-      </c>
-      <c r="C70" t="s">
-        <v>346</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="D73" t="s">
         <v>347</v>
       </c>
-      <c r="E70" s="7">
-        <v>1</v>
-      </c>
-      <c r="F70" t="s">
+      <c r="E73" s="7">
+        <v>1</v>
+      </c>
+      <c r="F73" s="24" t="s">
         <v>340</v>
       </c>
-      <c r="G70" s="6">
-        <v>129.94999999999999</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="A71" s="4" t="s">
-        <v>338</v>
-      </c>
-      <c r="C71" t="s">
-        <v>346</v>
-      </c>
-      <c r="D71" t="s">
-        <v>348</v>
-      </c>
-      <c r="E71" s="7">
-        <v>1</v>
-      </c>
-      <c r="F71" s="24" t="s">
-        <v>341</v>
-      </c>
-      <c r="G71" s="6">
+      <c r="G73" s="6">
         <v>129</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="G72" s="19"/>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G74" s="19"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:B3">
@@ -3553,9 +3599,9 @@
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink ref="C55" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="F63" r:id="rId2" xr:uid="{67448854-A366-4062-8C25-6B79CA0C5B75}"/>
-    <hyperlink ref="C56" r:id="rId3" xr:uid="{01278BAA-72A8-4F07-B69E-698B3A7AE6BF}"/>
+    <hyperlink ref="C57" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F65" r:id="rId2" xr:uid="{67448854-A366-4062-8C25-6B79CA0C5B75}"/>
+    <hyperlink ref="C58" r:id="rId3" xr:uid="{01278BAA-72A8-4F07-B69E-698B3A7AE6BF}"/>
   </hyperlinks>
   <printOptions gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4077,16 +4123,16 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="25" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B1" s="26" t="s">
         <v>140</v>
       </c>
       <c r="C1" s="33" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1" s="26" t="s">
         <v>367</v>
-      </c>
-      <c r="D1" s="26" t="s">
-        <v>368</v>
       </c>
       <c r="F1" t="s">
         <v>142</v>
@@ -4121,35 +4167,35 @@
     </row>
     <row r="2" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="31" t="s">
+        <v>368</v>
+      </c>
+      <c r="B2" s="28" t="s">
         <v>369</v>
-      </c>
-      <c r="B2" s="28" t="s">
-        <v>370</v>
       </c>
       <c r="C2" s="34">
         <v>28</v>
       </c>
       <c r="D2" s="28" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="27" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B3" s="28" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C3" s="34">
         <v>1</v>
       </c>
       <c r="D3" s="28" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="29" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B4" s="30" t="s">
         <v>159</v>
@@ -4158,12 +4204,12 @@
         <v>2</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="29" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B5" s="30" t="s">
         <v>183</v>
@@ -4172,12 +4218,12 @@
         <v>2</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="29" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B6" s="30" t="s">
         <v>183</v>
@@ -4186,7 +4232,7 @@
         <v>2</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.35">
@@ -4200,12 +4246,12 @@
         <v>1</v>
       </c>
       <c r="D7" s="28" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="32" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B8" s="30" t="s">
         <v>183</v>
@@ -4214,12 +4260,12 @@
         <v>24</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="29" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B9" s="30" t="s">
         <v>183</v>
@@ -4228,7 +4274,7 @@
         <v>4</v>
       </c>
       <c r="D9" s="30" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
@@ -4242,12 +4288,12 @@
         <v>1</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="27" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B11" s="28" t="s">
         <v>183</v>
@@ -4256,7 +4302,7 @@
         <v>3</v>
       </c>
       <c r="D11" s="28" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.35">
@@ -4270,7 +4316,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.35">
@@ -4284,12 +4330,12 @@
         <v>1</v>
       </c>
       <c r="D13" s="30" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="27" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B14" s="28" t="s">
         <v>153</v>
@@ -4303,7 +4349,7 @@
     </row>
     <row r="15" spans="1:15" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A15" s="32" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>162</v>
@@ -4312,12 +4358,12 @@
         <v>16</v>
       </c>
       <c r="D15" s="30" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="27" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B16" s="28" t="s">
         <v>188</v>
@@ -4354,7 +4400,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="28" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.35">
@@ -4362,13 +4408,13 @@
         <v>186</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C19" s="35">
         <v>1</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.35">
@@ -4396,7 +4442,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="28" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.35">
@@ -4410,7 +4456,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.35">
@@ -4424,12 +4470,12 @@
         <v>1</v>
       </c>
       <c r="D23" s="28" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A24" s="27" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B24" s="28" t="s">
         <v>161</v>
@@ -4452,12 +4498,12 @@
         <v>1</v>
       </c>
       <c r="D25" s="28" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="27" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B26" s="28" t="s">
         <v>73</v>
@@ -4466,7 +4512,7 @@
         <v>1</v>
       </c>
       <c r="D26" s="28" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.35">
@@ -4480,12 +4526,12 @@
         <v>1</v>
       </c>
       <c r="D27" s="30" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28" s="29" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B28" s="30" t="s">
         <v>155</v>
@@ -4499,30 +4545,30 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29" s="29" t="s">
+        <v>384</v>
+      </c>
+      <c r="B29" s="30" t="s">
         <v>385</v>
       </c>
-      <c r="B29" s="30" t="s">
-        <v>386</v>
-      </c>
       <c r="C29" s="35">
         <v>1</v>
       </c>
       <c r="D29" s="30" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="29" t="s">
+        <v>386</v>
+      </c>
+      <c r="B30" s="30" t="s">
         <v>387</v>
       </c>
-      <c r="B30" s="30" t="s">
-        <v>388</v>
-      </c>
       <c r="C30" s="35">
         <v>1</v>
       </c>
       <c r="D30" s="30" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.35">
@@ -4536,7 +4582,7 @@
         <v>1</v>
       </c>
       <c r="D31" s="28" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>